<commit_message>
Maintain ETL Test Framework for Hive database
</commit_message>
<xml_diff>
--- a/src/main/resources/input-excel-file/schema/HIVE_INTF_SCHEMA.xlsx
+++ b/src/main/resources/input-excel-file/schema/HIVE_INTF_SCHEMA.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutoData\data-etl-reconcilation\src\main\resources\input-excel-file\schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4A9C94C-6801-41DF-8E3A-2077C2A0173E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B49815F-D3D9-4EFB-AE1E-8D2E377699A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CYC_INTF" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -937,10 +937,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
DP-610: LN_INTF gererate test scripts
</commit_message>
<xml_diff>
--- a/src/main/resources/input-excel-file/schema/HIVE_INTF_SCHEMA.xlsx
+++ b/src/main/resources/input-excel-file/schema/HIVE_INTF_SCHEMA.xlsx
@@ -5,22 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutoData\data-etl-reconcilation\src\main\resources\input-excel-file\schema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code ETL frame work\data-etl-reconcilation\src\main\resources\input-excel-file\schema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B49815F-D3D9-4EFB-AE1E-8D2E377699A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17494BFB-F37F-40DF-9AB5-7D6F552EE58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CYC_INTF" sheetId="1" r:id="rId1"/>
+    <sheet name="LN_INTF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
   <si>
     <t>col_name</t>
   </si>
@@ -98,6 +112,36 @@
   </si>
   <si>
     <t># col_name</t>
+  </si>
+  <si>
+    <t>ln_anchor_id</t>
+  </si>
+  <si>
+    <t>toll_id</t>
+  </si>
+  <si>
+    <t>ln_code</t>
+  </si>
+  <si>
+    <t>ln_nm</t>
+  </si>
+  <si>
+    <t>ln_tp</t>
+  </si>
+  <si>
+    <t>ln_stt</t>
+  </si>
+  <si>
+    <t>DECIMAL</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>BIGINT</t>
+  </si>
+  <si>
+    <t>INT</t>
   </si>
 </sst>
 </file>
@@ -941,7 +985,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1124,4 +1168,210 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCB25AC-9AEA-4911-979D-5EC137B81662}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>